<commit_message>
modified baseline results for garbage values/rounding
</commit_message>
<xml_diff>
--- a/Tests/baseline_sma_5_25_DDD.xlsx
+++ b/Tests/baseline_sma_5_25_DDD.xlsx
@@ -8,24 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Windows\Documents\bt_plat\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2394563-9B7D-43CF-B4CF-8D91B4EA3D6A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F41896-521C-4F79-9B75-FEAC8C147DC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tests" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="22">
   <si>
     <t>Symbol</t>
   </si>
@@ -88,6 +95,9 @@
   </si>
   <si>
     <t>Open Long</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -409,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:R51"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3068,4 +3078,2029 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABA09DD1-E115-47F2-A5F6-8E6DFAD31422}">
+  <dimension ref="A1:P50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1">
+        <v>40717</v>
+      </c>
+      <c r="D2">
+        <v>12.83</v>
+      </c>
+      <c r="E2" s="1">
+        <v>40756</v>
+      </c>
+      <c r="F2">
+        <v>13.95</v>
+      </c>
+      <c r="G2" s="2">
+        <v>8.7300000000000003E-2</v>
+      </c>
+      <c r="H2">
+        <v>86.24</v>
+      </c>
+      <c r="I2" s="2">
+        <v>8.7300000000000003E-2</v>
+      </c>
+      <c r="J2">
+        <v>77</v>
+      </c>
+      <c r="K2">
+        <v>987.91</v>
+      </c>
+      <c r="L2">
+        <v>86.24</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1">
+        <v>40787</v>
+      </c>
+      <c r="D3">
+        <v>11.5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>40792</v>
+      </c>
+      <c r="F3">
+        <v>10.64</v>
+      </c>
+      <c r="G3" s="2">
+        <v>-7.4800000000000005E-2</v>
+      </c>
+      <c r="H3">
+        <v>-74.819999999999993</v>
+      </c>
+      <c r="I3" s="2">
+        <v>-7.4800000000000005E-2</v>
+      </c>
+      <c r="J3">
+        <v>87</v>
+      </c>
+      <c r="K3">
+        <v>1000.5</v>
+      </c>
+      <c r="L3">
+        <v>11.42</v>
+      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1">
+        <v>40827</v>
+      </c>
+      <c r="D4">
+        <v>11.39</v>
+      </c>
+      <c r="E4" s="1">
+        <v>40849</v>
+      </c>
+      <c r="F4">
+        <v>10.75</v>
+      </c>
+      <c r="G4" s="2">
+        <v>-5.62E-2</v>
+      </c>
+      <c r="H4">
+        <v>-55.68</v>
+      </c>
+      <c r="I4" s="2">
+        <v>-5.62E-2</v>
+      </c>
+      <c r="J4">
+        <v>87</v>
+      </c>
+      <c r="K4">
+        <v>990.93</v>
+      </c>
+      <c r="L4">
+        <v>-44.26</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1">
+        <v>40914</v>
+      </c>
+      <c r="D5">
+        <v>10.67</v>
+      </c>
+      <c r="E5" s="1">
+        <v>41044</v>
+      </c>
+      <c r="F5">
+        <v>18.28</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.71319999999999995</v>
+      </c>
+      <c r="H5">
+        <v>707.73</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.71319999999999995</v>
+      </c>
+      <c r="J5">
+        <v>93</v>
+      </c>
+      <c r="K5">
+        <v>992.31</v>
+      </c>
+      <c r="L5">
+        <v>663.47</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1">
+        <v>41054</v>
+      </c>
+      <c r="D6">
+        <v>20.420000000000002</v>
+      </c>
+      <c r="E6" s="1">
+        <v>41163</v>
+      </c>
+      <c r="F6">
+        <v>26.11</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.27860000000000001</v>
+      </c>
+      <c r="H6">
+        <v>295.88</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.27860000000000001</v>
+      </c>
+      <c r="J6">
+        <v>52</v>
+      </c>
+      <c r="K6">
+        <v>1061.8399999999999</v>
+      </c>
+      <c r="L6">
+        <v>959.35</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1">
+        <v>41198</v>
+      </c>
+      <c r="D7">
+        <v>26.61</v>
+      </c>
+      <c r="E7" s="1">
+        <v>41229</v>
+      </c>
+      <c r="F7">
+        <v>25.36</v>
+      </c>
+      <c r="G7" s="2">
+        <v>-4.7E-2</v>
+      </c>
+      <c r="H7">
+        <v>-51.25</v>
+      </c>
+      <c r="I7" s="2">
+        <v>-4.7E-2</v>
+      </c>
+      <c r="J7">
+        <v>41</v>
+      </c>
+      <c r="K7">
+        <v>1091.01</v>
+      </c>
+      <c r="L7">
+        <v>908.1</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1">
+        <v>41239</v>
+      </c>
+      <c r="D8">
+        <v>31.03</v>
+      </c>
+      <c r="E8" s="1">
+        <v>41306</v>
+      </c>
+      <c r="F8">
+        <v>39.03</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.25779999999999997</v>
+      </c>
+      <c r="H8">
+        <v>280</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.25779999999999997</v>
+      </c>
+      <c r="J8">
+        <v>35</v>
+      </c>
+      <c r="K8">
+        <v>1086.05</v>
+      </c>
+      <c r="L8">
+        <v>1188.0999999999999</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1">
+        <v>41312</v>
+      </c>
+      <c r="D9">
+        <v>44.03</v>
+      </c>
+      <c r="E9" s="1">
+        <v>41324</v>
+      </c>
+      <c r="F9">
+        <v>40.130000000000003</v>
+      </c>
+      <c r="G9" s="2">
+        <v>-8.8599999999999998E-2</v>
+      </c>
+      <c r="H9">
+        <v>-97.5</v>
+      </c>
+      <c r="I9" s="2">
+        <v>-8.8599999999999998E-2</v>
+      </c>
+      <c r="J9">
+        <v>25</v>
+      </c>
+      <c r="K9">
+        <v>1100.75</v>
+      </c>
+      <c r="L9">
+        <v>1090.5999999999999</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1">
+        <v>41374</v>
+      </c>
+      <c r="D10">
+        <v>34.44</v>
+      </c>
+      <c r="E10" s="1">
+        <v>41432</v>
+      </c>
+      <c r="F10">
+        <v>45.23</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.31330000000000002</v>
+      </c>
+      <c r="H10">
+        <v>345.28</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.31330000000000002</v>
+      </c>
+      <c r="J10">
+        <v>32</v>
+      </c>
+      <c r="K10">
+        <v>1102.08</v>
+      </c>
+      <c r="L10">
+        <v>1435.88</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1">
+        <v>41443</v>
+      </c>
+      <c r="D11">
+        <v>47.78</v>
+      </c>
+      <c r="E11" s="1">
+        <v>41446</v>
+      </c>
+      <c r="F11">
+        <v>43.5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>-8.9599999999999999E-2</v>
+      </c>
+      <c r="H11">
+        <v>-98.44</v>
+      </c>
+      <c r="I11" s="2">
+        <v>-8.9599999999999999E-2</v>
+      </c>
+      <c r="J11">
+        <v>23</v>
+      </c>
+      <c r="K11">
+        <v>1098.94</v>
+      </c>
+      <c r="L11">
+        <v>1337.44</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1">
+        <v>41463</v>
+      </c>
+      <c r="D12">
+        <v>46.31</v>
+      </c>
+      <c r="E12" s="1">
+        <v>41492</v>
+      </c>
+      <c r="F12">
+        <v>46.3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>-2.0000000000000001E-4</v>
+      </c>
+      <c r="H12">
+        <v>-0.24</v>
+      </c>
+      <c r="I12" s="2">
+        <v>-2.0000000000000001E-4</v>
+      </c>
+      <c r="J12">
+        <v>24</v>
+      </c>
+      <c r="K12">
+        <v>1111.44</v>
+      </c>
+      <c r="L12">
+        <v>1337.2</v>
+      </c>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1">
+        <v>41499</v>
+      </c>
+      <c r="D13">
+        <v>49.21</v>
+      </c>
+      <c r="E13" s="1">
+        <v>41505</v>
+      </c>
+      <c r="F13">
+        <v>46.77</v>
+      </c>
+      <c r="G13" s="2">
+        <v>-4.9599999999999998E-2</v>
+      </c>
+      <c r="H13">
+        <v>-56.12</v>
+      </c>
+      <c r="I13" s="2">
+        <v>-4.9599999999999998E-2</v>
+      </c>
+      <c r="J13">
+        <v>23</v>
+      </c>
+      <c r="K13">
+        <v>1131.83</v>
+      </c>
+      <c r="L13">
+        <v>1281.08</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1">
+        <v>41509</v>
+      </c>
+      <c r="D14">
+        <v>48.44</v>
+      </c>
+      <c r="E14" s="1">
+        <v>41556</v>
+      </c>
+      <c r="F14">
+        <v>49.46</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="H14">
+        <v>23.46</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="J14">
+        <v>23</v>
+      </c>
+      <c r="K14">
+        <v>1114.1199999999999</v>
+      </c>
+      <c r="L14">
+        <v>1304.54</v>
+      </c>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1">
+        <v>41563</v>
+      </c>
+      <c r="D15">
+        <v>55.25</v>
+      </c>
+      <c r="E15" s="1">
+        <v>41661</v>
+      </c>
+      <c r="F15">
+        <v>88.26</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.59750000000000003</v>
+      </c>
+      <c r="H15">
+        <v>660.2</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.59750000000000003</v>
+      </c>
+      <c r="J15">
+        <v>20</v>
+      </c>
+      <c r="K15">
+        <v>1105</v>
+      </c>
+      <c r="L15">
+        <v>1964.74</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="1">
+        <v>41691</v>
+      </c>
+      <c r="D16">
+        <v>80.739999999999995</v>
+      </c>
+      <c r="E16" s="1">
+        <v>41704</v>
+      </c>
+      <c r="F16">
+        <v>68.5</v>
+      </c>
+      <c r="G16" s="2">
+        <v>-0.15160000000000001</v>
+      </c>
+      <c r="H16">
+        <v>-171.36</v>
+      </c>
+      <c r="I16" s="2">
+        <v>-0.15160000000000001</v>
+      </c>
+      <c r="J16">
+        <v>14</v>
+      </c>
+      <c r="K16">
+        <v>1130.3599999999999</v>
+      </c>
+      <c r="L16">
+        <v>1793.38</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1">
+        <v>41775</v>
+      </c>
+      <c r="D17">
+        <v>48.37</v>
+      </c>
+      <c r="E17" s="1">
+        <v>41779</v>
+      </c>
+      <c r="F17">
+        <v>49.32</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="H17">
+        <v>22.8</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="J17">
+        <v>24</v>
+      </c>
+      <c r="K17">
+        <v>1160.8800000000001</v>
+      </c>
+      <c r="L17">
+        <v>1816.18</v>
+      </c>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1">
+        <v>41780</v>
+      </c>
+      <c r="D18">
+        <v>50.78</v>
+      </c>
+      <c r="E18" s="1">
+        <v>41799</v>
+      </c>
+      <c r="F18">
+        <v>50.16</v>
+      </c>
+      <c r="G18" s="2">
+        <v>-1.2200000000000001E-2</v>
+      </c>
+      <c r="H18">
+        <v>-14.26</v>
+      </c>
+      <c r="I18" s="2">
+        <v>-1.2200000000000001E-2</v>
+      </c>
+      <c r="J18">
+        <v>23</v>
+      </c>
+      <c r="K18">
+        <v>1167.94</v>
+      </c>
+      <c r="L18">
+        <v>1801.92</v>
+      </c>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1">
+        <v>41808</v>
+      </c>
+      <c r="D19">
+        <v>53.7</v>
+      </c>
+      <c r="E19" s="1">
+        <v>41841</v>
+      </c>
+      <c r="F19">
+        <v>56.6</v>
+      </c>
+      <c r="G19" s="2">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="H19">
+        <v>60.9</v>
+      </c>
+      <c r="I19" s="2">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="J19">
+        <v>21</v>
+      </c>
+      <c r="K19">
+        <v>1127.7</v>
+      </c>
+      <c r="L19">
+        <v>1862.82</v>
+      </c>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1">
+        <v>41877</v>
+      </c>
+      <c r="D20">
+        <v>51.44</v>
+      </c>
+      <c r="E20" s="1">
+        <v>41900</v>
+      </c>
+      <c r="F20">
+        <v>50.32</v>
+      </c>
+      <c r="G20" s="2">
+        <v>-2.18E-2</v>
+      </c>
+      <c r="H20">
+        <v>-25.76</v>
+      </c>
+      <c r="I20" s="2">
+        <v>-2.18E-2</v>
+      </c>
+      <c r="J20">
+        <v>23</v>
+      </c>
+      <c r="K20">
+        <v>1183.1199999999999</v>
+      </c>
+      <c r="L20">
+        <v>1837.06</v>
+      </c>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="1">
+        <v>41968</v>
+      </c>
+      <c r="D21">
+        <v>36.869999999999997</v>
+      </c>
+      <c r="E21" s="1">
+        <v>41974</v>
+      </c>
+      <c r="F21">
+        <v>33.57</v>
+      </c>
+      <c r="G21" s="2">
+        <v>-8.9499999999999996E-2</v>
+      </c>
+      <c r="H21">
+        <v>-105.6</v>
+      </c>
+      <c r="I21" s="2">
+        <v>-8.9499999999999996E-2</v>
+      </c>
+      <c r="J21">
+        <v>32</v>
+      </c>
+      <c r="K21">
+        <v>1179.8399999999999</v>
+      </c>
+      <c r="L21">
+        <v>1731.46</v>
+      </c>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="1">
+        <v>42006</v>
+      </c>
+      <c r="D22">
+        <v>32.42</v>
+      </c>
+      <c r="E22" s="1">
+        <v>42009</v>
+      </c>
+      <c r="F22">
+        <v>30.74</v>
+      </c>
+      <c r="G22" s="2">
+        <v>-5.1799999999999999E-2</v>
+      </c>
+      <c r="H22">
+        <v>-60.48</v>
+      </c>
+      <c r="I22" s="2">
+        <v>-5.1799999999999999E-2</v>
+      </c>
+      <c r="J22">
+        <v>36</v>
+      </c>
+      <c r="K22">
+        <v>1167.1199999999999</v>
+      </c>
+      <c r="L22">
+        <v>1670.98</v>
+      </c>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="1">
+        <v>42017</v>
+      </c>
+      <c r="D23">
+        <v>30.88</v>
+      </c>
+      <c r="E23" s="1">
+        <v>42019</v>
+      </c>
+      <c r="F23">
+        <v>28.33</v>
+      </c>
+      <c r="G23" s="2">
+        <v>-8.2600000000000007E-2</v>
+      </c>
+      <c r="H23">
+        <v>-94.35</v>
+      </c>
+      <c r="I23" s="2">
+        <v>-8.2600000000000007E-2</v>
+      </c>
+      <c r="J23">
+        <v>37</v>
+      </c>
+      <c r="K23">
+        <v>1142.56</v>
+      </c>
+      <c r="L23">
+        <v>1576.63</v>
+      </c>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="1">
+        <v>42047</v>
+      </c>
+      <c r="D24">
+        <v>32.409999999999997</v>
+      </c>
+      <c r="E24" s="1">
+        <v>42066</v>
+      </c>
+      <c r="F24">
+        <v>29.25</v>
+      </c>
+      <c r="G24" s="2">
+        <v>-9.7500000000000003E-2</v>
+      </c>
+      <c r="H24">
+        <v>-110.6</v>
+      </c>
+      <c r="I24" s="2">
+        <v>-9.7500000000000003E-2</v>
+      </c>
+      <c r="J24">
+        <v>35</v>
+      </c>
+      <c r="K24">
+        <v>1134.3499999999999</v>
+      </c>
+      <c r="L24">
+        <v>1466.03</v>
+      </c>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="1">
+        <v>42101</v>
+      </c>
+      <c r="D25">
+        <v>28.35</v>
+      </c>
+      <c r="E25" s="1">
+        <v>42121</v>
+      </c>
+      <c r="F25">
+        <v>25.28</v>
+      </c>
+      <c r="G25" s="2">
+        <v>-0.10829999999999999</v>
+      </c>
+      <c r="H25">
+        <v>-122.8</v>
+      </c>
+      <c r="I25" s="2">
+        <v>-0.10829999999999999</v>
+      </c>
+      <c r="J25">
+        <v>40</v>
+      </c>
+      <c r="K25">
+        <v>1134</v>
+      </c>
+      <c r="L25">
+        <v>1343.23</v>
+      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="1">
+        <v>42249</v>
+      </c>
+      <c r="D26">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1">
+        <v>42255</v>
+      </c>
+      <c r="F26">
+        <v>13.3</v>
+      </c>
+      <c r="G26" s="2">
+        <v>2.3099999999999999E-2</v>
+      </c>
+      <c r="H26">
+        <v>26.1</v>
+      </c>
+      <c r="I26" s="2">
+        <v>2.3099999999999999E-2</v>
+      </c>
+      <c r="J26">
+        <v>87</v>
+      </c>
+      <c r="K26">
+        <v>1131</v>
+      </c>
+      <c r="L26">
+        <v>1369.33</v>
+      </c>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="1">
+        <v>42285</v>
+      </c>
+      <c r="D27">
+        <v>13.75</v>
+      </c>
+      <c r="E27" s="1">
+        <v>42298</v>
+      </c>
+      <c r="F27">
+        <v>12.09</v>
+      </c>
+      <c r="G27" s="2">
+        <v>-0.1207</v>
+      </c>
+      <c r="H27">
+        <v>-136.12</v>
+      </c>
+      <c r="I27" s="2">
+        <v>-0.1207</v>
+      </c>
+      <c r="J27">
+        <v>82</v>
+      </c>
+      <c r="K27">
+        <v>1127.5</v>
+      </c>
+      <c r="L27">
+        <v>1233.21</v>
+      </c>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="1">
+        <v>42348</v>
+      </c>
+      <c r="D28">
+        <v>9.65</v>
+      </c>
+      <c r="E28" s="1">
+        <v>42369</v>
+      </c>
+      <c r="F28">
+        <v>8.69</v>
+      </c>
+      <c r="G28" s="2">
+        <v>-9.9500000000000005E-2</v>
+      </c>
+      <c r="H28">
+        <v>-111.36</v>
+      </c>
+      <c r="I28" s="2">
+        <v>-9.9500000000000005E-2</v>
+      </c>
+      <c r="J28">
+        <v>116</v>
+      </c>
+      <c r="K28">
+        <v>1119.4000000000001</v>
+      </c>
+      <c r="L28">
+        <v>1121.8499999999999</v>
+      </c>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="1">
+        <v>42404</v>
+      </c>
+      <c r="D29">
+        <v>9.1300000000000008</v>
+      </c>
+      <c r="E29" s="1">
+        <v>42494</v>
+      </c>
+      <c r="F29">
+        <v>14.51</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.58930000000000005</v>
+      </c>
+      <c r="H29">
+        <v>650.98</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.58930000000000005</v>
+      </c>
+      <c r="J29">
+        <v>121</v>
+      </c>
+      <c r="K29">
+        <v>1104.73</v>
+      </c>
+      <c r="L29">
+        <v>1772.83</v>
+      </c>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="1">
+        <v>42524</v>
+      </c>
+      <c r="D30">
+        <v>13.55</v>
+      </c>
+      <c r="E30" s="1">
+        <v>42535</v>
+      </c>
+      <c r="F30">
+        <v>12.56</v>
+      </c>
+      <c r="G30" s="2">
+        <v>-7.3099999999999998E-2</v>
+      </c>
+      <c r="H30">
+        <v>-85.14</v>
+      </c>
+      <c r="I30" s="2">
+        <v>-7.3099999999999998E-2</v>
+      </c>
+      <c r="J30">
+        <v>86</v>
+      </c>
+      <c r="K30">
+        <v>1165.3</v>
+      </c>
+      <c r="L30">
+        <v>1687.69</v>
+      </c>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="1">
+        <v>42542</v>
+      </c>
+      <c r="D31">
+        <v>13.6</v>
+      </c>
+      <c r="E31" s="1">
+        <v>42548</v>
+      </c>
+      <c r="F31">
+        <v>11.67</v>
+      </c>
+      <c r="G31" s="2">
+        <v>-0.1419</v>
+      </c>
+      <c r="H31">
+        <v>-164.05</v>
+      </c>
+      <c r="I31" s="2">
+        <v>-0.1419</v>
+      </c>
+      <c r="J31">
+        <v>85</v>
+      </c>
+      <c r="K31">
+        <v>1156</v>
+      </c>
+      <c r="L31">
+        <v>1523.64</v>
+      </c>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="1">
+        <v>42557</v>
+      </c>
+      <c r="D32">
+        <v>13.19</v>
+      </c>
+      <c r="E32" s="1">
+        <v>42573</v>
+      </c>
+      <c r="F32">
+        <v>13.3</v>
+      </c>
+      <c r="G32" s="2">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="H32">
+        <v>9.57</v>
+      </c>
+      <c r="I32" s="2">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="J32">
+        <v>87</v>
+      </c>
+      <c r="K32">
+        <v>1147.53</v>
+      </c>
+      <c r="L32">
+        <v>1533.21</v>
+      </c>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="1">
+        <v>42587</v>
+      </c>
+      <c r="D33">
+        <v>14.77</v>
+      </c>
+      <c r="E33" s="1">
+        <v>42619</v>
+      </c>
+      <c r="F33">
+        <v>15.75</v>
+      </c>
+      <c r="G33" s="2">
+        <v>6.6400000000000001E-2</v>
+      </c>
+      <c r="H33">
+        <v>76.44</v>
+      </c>
+      <c r="I33" s="2">
+        <v>6.6400000000000001E-2</v>
+      </c>
+      <c r="J33">
+        <v>78</v>
+      </c>
+      <c r="K33">
+        <v>1152.06</v>
+      </c>
+      <c r="L33">
+        <v>1609.65</v>
+      </c>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="1">
+        <v>42625</v>
+      </c>
+      <c r="D34">
+        <v>15.49</v>
+      </c>
+      <c r="E34" s="1">
+        <v>42626</v>
+      </c>
+      <c r="F34">
+        <v>15.16</v>
+      </c>
+      <c r="G34" s="2">
+        <v>-2.1299999999999999E-2</v>
+      </c>
+      <c r="H34">
+        <v>-24.42</v>
+      </c>
+      <c r="I34" s="2">
+        <v>-2.1299999999999999E-2</v>
+      </c>
+      <c r="J34">
+        <v>74</v>
+      </c>
+      <c r="K34">
+        <v>1146.26</v>
+      </c>
+      <c r="L34">
+        <v>1585.23</v>
+      </c>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="1">
+        <v>42629</v>
+      </c>
+      <c r="D35">
+        <v>15.82</v>
+      </c>
+      <c r="E35" s="1">
+        <v>42656</v>
+      </c>
+      <c r="F35">
+        <v>14.82</v>
+      </c>
+      <c r="G35" s="2">
+        <v>-6.3200000000000006E-2</v>
+      </c>
+      <c r="H35">
+        <v>-73</v>
+      </c>
+      <c r="I35" s="2">
+        <v>-6.3200000000000006E-2</v>
+      </c>
+      <c r="J35">
+        <v>73</v>
+      </c>
+      <c r="K35">
+        <v>1154.8599999999999</v>
+      </c>
+      <c r="L35">
+        <v>1512.23</v>
+      </c>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="1">
+        <v>42689</v>
+      </c>
+      <c r="D36">
+        <v>13.91</v>
+      </c>
+      <c r="E36" s="1">
+        <v>42706</v>
+      </c>
+      <c r="F36">
+        <v>13.54</v>
+      </c>
+      <c r="G36" s="2">
+        <v>-2.6599999999999999E-2</v>
+      </c>
+      <c r="H36">
+        <v>-30.34</v>
+      </c>
+      <c r="I36" s="2">
+        <v>-2.6599999999999999E-2</v>
+      </c>
+      <c r="J36">
+        <v>82</v>
+      </c>
+      <c r="K36">
+        <v>1140.6199999999999</v>
+      </c>
+      <c r="L36">
+        <v>1481.89</v>
+      </c>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="1">
+        <v>42710</v>
+      </c>
+      <c r="D37">
+        <v>15.15</v>
+      </c>
+      <c r="E37" s="1">
+        <v>42727</v>
+      </c>
+      <c r="F37">
+        <v>14.23</v>
+      </c>
+      <c r="G37" s="2">
+        <v>-6.0699999999999997E-2</v>
+      </c>
+      <c r="H37">
+        <v>-69</v>
+      </c>
+      <c r="I37" s="2">
+        <v>-6.0699999999999997E-2</v>
+      </c>
+      <c r="J37">
+        <v>75</v>
+      </c>
+      <c r="K37">
+        <v>1136.25</v>
+      </c>
+      <c r="L37">
+        <v>1412.89</v>
+      </c>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="1">
+        <v>42744</v>
+      </c>
+      <c r="D38">
+        <v>16.73</v>
+      </c>
+      <c r="E38" s="1">
+        <v>42793</v>
+      </c>
+      <c r="F38">
+        <v>16.940000000000001</v>
+      </c>
+      <c r="G38" s="2">
+        <v>1.26E-2</v>
+      </c>
+      <c r="H38">
+        <v>14.28</v>
+      </c>
+      <c r="I38" s="2">
+        <v>1.26E-2</v>
+      </c>
+      <c r="J38">
+        <v>68</v>
+      </c>
+      <c r="K38">
+        <v>1137.6400000000001</v>
+      </c>
+      <c r="L38">
+        <v>1427.17</v>
+      </c>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="1">
+        <v>42825</v>
+      </c>
+      <c r="D39">
+        <v>14.96</v>
+      </c>
+      <c r="E39" s="1">
+        <v>42835</v>
+      </c>
+      <c r="F39">
+        <v>14.29</v>
+      </c>
+      <c r="G39" s="2">
+        <v>-4.48E-2</v>
+      </c>
+      <c r="H39">
+        <v>-50.92</v>
+      </c>
+      <c r="I39" s="2">
+        <v>-4.48E-2</v>
+      </c>
+      <c r="J39">
+        <v>76</v>
+      </c>
+      <c r="K39">
+        <v>1136.96</v>
+      </c>
+      <c r="L39">
+        <v>1376.25</v>
+      </c>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="1">
+        <v>42842</v>
+      </c>
+      <c r="D40">
+        <v>14.88</v>
+      </c>
+      <c r="E40" s="1">
+        <v>42893</v>
+      </c>
+      <c r="F40">
+        <v>20.74</v>
+      </c>
+      <c r="G40" s="2">
+        <v>0.39379999999999998</v>
+      </c>
+      <c r="H40">
+        <v>445.36</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0.39379999999999998</v>
+      </c>
+      <c r="J40">
+        <v>76</v>
+      </c>
+      <c r="K40">
+        <v>1130.8800000000001</v>
+      </c>
+      <c r="L40">
+        <v>1821.61</v>
+      </c>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="1">
+        <v>42907</v>
+      </c>
+      <c r="D41">
+        <v>21.69</v>
+      </c>
+      <c r="E41" s="1">
+        <v>42915</v>
+      </c>
+      <c r="F41">
+        <v>20.190000000000001</v>
+      </c>
+      <c r="G41" s="2">
+        <v>-6.9199999999999998E-2</v>
+      </c>
+      <c r="H41">
+        <v>-81</v>
+      </c>
+      <c r="I41" s="2">
+        <v>-6.9199999999999998E-2</v>
+      </c>
+      <c r="J41">
+        <v>54</v>
+      </c>
+      <c r="K41">
+        <v>1171.26</v>
+      </c>
+      <c r="L41">
+        <v>1740.61</v>
+      </c>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="1">
+        <v>42984</v>
+      </c>
+      <c r="D42">
+        <v>13.09</v>
+      </c>
+      <c r="E42" s="1">
+        <v>43018</v>
+      </c>
+      <c r="F42">
+        <v>12.68</v>
+      </c>
+      <c r="G42" s="2">
+        <v>-3.1300000000000001E-2</v>
+      </c>
+      <c r="H42">
+        <v>-36.49</v>
+      </c>
+      <c r="I42" s="2">
+        <v>-3.1300000000000001E-2</v>
+      </c>
+      <c r="J42">
+        <v>89</v>
+      </c>
+      <c r="K42">
+        <v>1165.01</v>
+      </c>
+      <c r="L42">
+        <v>1704.12</v>
+      </c>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="1">
+        <v>43074</v>
+      </c>
+      <c r="D43">
+        <v>9.61</v>
+      </c>
+      <c r="E43" s="1">
+        <v>43097</v>
+      </c>
+      <c r="F43">
+        <v>8.76</v>
+      </c>
+      <c r="G43" s="2">
+        <v>-8.8400000000000006E-2</v>
+      </c>
+      <c r="H43">
+        <v>-102.85</v>
+      </c>
+      <c r="I43" s="2">
+        <v>-8.8400000000000006E-2</v>
+      </c>
+      <c r="J43">
+        <v>121</v>
+      </c>
+      <c r="K43">
+        <v>1162.81</v>
+      </c>
+      <c r="L43">
+        <v>1601.27</v>
+      </c>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="1">
+        <v>43111</v>
+      </c>
+      <c r="D44">
+        <v>10.29</v>
+      </c>
+      <c r="E44" s="1">
+        <v>43136</v>
+      </c>
+      <c r="F44">
+        <v>9.07</v>
+      </c>
+      <c r="G44" s="2">
+        <v>-0.1186</v>
+      </c>
+      <c r="H44">
+        <v>-136.63999999999999</v>
+      </c>
+      <c r="I44" s="2">
+        <v>-0.1186</v>
+      </c>
+      <c r="J44">
+        <v>112</v>
+      </c>
+      <c r="K44">
+        <v>1152.48</v>
+      </c>
+      <c r="L44">
+        <v>1464.63</v>
+      </c>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="1">
+        <v>43157</v>
+      </c>
+      <c r="D45">
+        <v>10.37</v>
+      </c>
+      <c r="E45" s="1">
+        <v>43159</v>
+      </c>
+      <c r="F45">
+        <v>9.5</v>
+      </c>
+      <c r="G45" s="2">
+        <v>-8.3900000000000002E-2</v>
+      </c>
+      <c r="H45">
+        <v>-95.7</v>
+      </c>
+      <c r="I45" s="2">
+        <v>-8.3900000000000002E-2</v>
+      </c>
+      <c r="J45">
+        <v>110</v>
+      </c>
+      <c r="K45">
+        <v>1140.7</v>
+      </c>
+      <c r="L45">
+        <v>1368.93</v>
+      </c>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="1">
+        <v>43160</v>
+      </c>
+      <c r="D46">
+        <v>10.74</v>
+      </c>
+      <c r="E46" s="1">
+        <v>43187</v>
+      </c>
+      <c r="F46">
+        <v>11.3</v>
+      </c>
+      <c r="G46" s="2">
+        <v>5.21E-2</v>
+      </c>
+      <c r="H46">
+        <v>58.8</v>
+      </c>
+      <c r="I46" s="2">
+        <v>5.21E-2</v>
+      </c>
+      <c r="J46">
+        <v>105</v>
+      </c>
+      <c r="K46">
+        <v>1127.7</v>
+      </c>
+      <c r="L46">
+        <v>1427.73</v>
+      </c>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="1">
+        <v>43203</v>
+      </c>
+      <c r="D47">
+        <v>11.93</v>
+      </c>
+      <c r="E47" s="1">
+        <v>43214</v>
+      </c>
+      <c r="F47">
+        <v>11.21</v>
+      </c>
+      <c r="G47" s="2">
+        <v>-6.0400000000000002E-2</v>
+      </c>
+      <c r="H47">
+        <v>-68.400000000000006</v>
+      </c>
+      <c r="I47" s="2">
+        <v>-6.0400000000000002E-2</v>
+      </c>
+      <c r="J47">
+        <v>95</v>
+      </c>
+      <c r="K47">
+        <v>1133.3499999999999</v>
+      </c>
+      <c r="L47">
+        <v>1359.33</v>
+      </c>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="1">
+        <v>43231</v>
+      </c>
+      <c r="D48">
+        <v>12.03</v>
+      </c>
+      <c r="E48" s="1">
+        <v>43283</v>
+      </c>
+      <c r="F48">
+        <v>14.09</v>
+      </c>
+      <c r="G48" s="2">
+        <v>0.17119999999999999</v>
+      </c>
+      <c r="H48">
+        <v>193.64</v>
+      </c>
+      <c r="I48" s="2">
+        <v>0.17119999999999999</v>
+      </c>
+      <c r="J48">
+        <v>94</v>
+      </c>
+      <c r="K48">
+        <v>1130.82</v>
+      </c>
+      <c r="L48">
+        <v>1552.97</v>
+      </c>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="1">
+        <v>43286</v>
+      </c>
+      <c r="D49">
+        <v>14.42</v>
+      </c>
+      <c r="E49" s="1">
+        <v>43307</v>
+      </c>
+      <c r="F49">
+        <v>13.17</v>
+      </c>
+      <c r="G49" s="2">
+        <v>-8.6699999999999999E-2</v>
+      </c>
+      <c r="H49">
+        <v>-100</v>
+      </c>
+      <c r="I49" s="2">
+        <v>-8.6699999999999999E-2</v>
+      </c>
+      <c r="J49">
+        <v>80</v>
+      </c>
+      <c r="K49">
+        <v>1153.5999999999999</v>
+      </c>
+      <c r="L49">
+        <v>1452.97</v>
+      </c>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" s="1">
+        <v>43321</v>
+      </c>
+      <c r="D50">
+        <v>18.16</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F50">
+        <v>17.920000000000002</v>
+      </c>
+      <c r="G50" s="2">
+        <v>-1.32E-2</v>
+      </c>
+      <c r="H50">
+        <v>-15.12</v>
+      </c>
+      <c r="I50" s="2">
+        <v>-1.32E-2</v>
+      </c>
+      <c r="J50">
+        <v>63</v>
+      </c>
+      <c r="K50">
+        <v>1144.08</v>
+      </c>
+      <c r="L50">
+        <v>1437.85</v>
+      </c>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>